<commit_message>
regresi bpjs kesehatan positive, kesehatan advice positive, kesehatan pu
</commit_message>
<xml_diff>
--- a/IOS/Bayar Beli - Paket Data XL/Default.xlsx
+++ b/IOS/Bayar Beli - Paket Data XL/Default.xlsx
@@ -4,11 +4,13 @@
   <fileVersion appName="SpreadsheetGear 8.2.5.102"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
     <sheet name="Paket Data XL - Positive" sheetId="2" r:id="rId2"/>
+    <sheet name="Paket Data XL - Negative" sheetId="3" r:id="rId3"/>
+    <sheet name="Pulsa XL - Positive" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>
@@ -549,7 +551,7 @@
     <col min="7" max="16384" width="8.8984375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1">
+    <row r="1" ht="14.95" customFormat="1">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -594,7 +596,7 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -603,7 +605,45 @@
     <col min="1" max="16384" width="8.8984375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customFormat="1"/>
+    <row r="1" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
regresi dan scripting paket data tri positive, paket data indosat positive
</commit_message>
<xml_diff>
--- a/IOS/Bayar Beli - Paket Data XL/Default.xlsx
+++ b/IOS/Bayar Beli - Paket Data XL/Default.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="SpreadsheetGear 8.2.5.102"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
     <sheet name="Paket Data XL - Positive" sheetId="2" r:id="rId2"/>
     <sheet name="Paket Data XL - Negative" sheetId="3" r:id="rId3"/>
     <sheet name="Pulsa XL - Positive" sheetId="4" r:id="rId4"/>
+    <sheet name="Pulsa XL - Negative" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>
@@ -229,10 +230,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -542,13 +543,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="10.75390625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.48828125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.37109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.3671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.4609375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.8984375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.75390625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.48828125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.37109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.3671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.4609375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.8984375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.95" customFormat="1">
@@ -572,17 +573,17 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="3"/>
@@ -602,7 +603,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.95"/>
   <cols>
-    <col min="1" max="16384" width="8.8984375" style="2" customWidth="1"/>
+    <col min="1" max="16384" width="8.8984375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1"/>
@@ -621,16 +622,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1"/>
+    <row r="1" ht="14.95" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.95" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
@@ -640,7 +660,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1"/>

</xml_diff>